<commit_message>
Update new device: THA0821ASW01
</commit_message>
<xml_diff>
--- a/DataCollection.xlsx
+++ b/DataCollection.xlsx
@@ -12,6 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LDG0158ASW01" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BNH0079ASW04 " sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DNG5031ASW09" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="THA0821ASW01" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
@@ -6278,4 +6279,1141 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Port</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>PVID</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>FlowControl</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>SpeedDuplex</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>t037_a_line_dinhbt1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>t037_a_line_tuha</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>100M</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>100-full</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>10/100/1000M</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>10/100/1000M</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>10/100/1000M</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>UPLINK_THA0821SRT03</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>10/100/1000M</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1000-full</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>